<commit_message>
update lk kelanis dan pcc
</commit_message>
<xml_diff>
--- a/Rekap LK/SSI-I.23.001 PCC Adaro/Rekap LK Adaro PCC (version 1).xlsx
+++ b/Rekap LK/SSI-I.23.001 PCC Adaro/Rekap LK Adaro PCC (version 1).xlsx
@@ -2457,10 +2457,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00"/>
     <numFmt numFmtId="181" formatCode="dd\-mmm\-yy"/>
@@ -2616,30 +2616,9 @@
       <charset val="134"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2653,17 +2632,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2678,7 +2648,60 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2692,19 +2715,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2718,43 +2754,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2797,7 +2797,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2809,7 +2839,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2821,19 +2893,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2845,13 +2929,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2869,79 +2947,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2959,25 +2965,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3254,30 +3254,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3317,6 +3293,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -3332,11 +3326,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3354,145 +3354,145 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="25" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="25" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="28" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="5" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3519,7 +3519,7 @@
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3556,7 +3556,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3567,7 +3567,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3575,7 +3575,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3584,7 +3584,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3652,21 +3652,21 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="178" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3685,8 +3685,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3747,7 +3747,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9924,7 +9924,7 @@
   <dimension ref="B3:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="16.5"/>
@@ -9988,7 +9988,7 @@
       </c>
       <c r="G5" s="14">
         <f>F37</f>
-        <v>311820035</v>
+        <v>311020035</v>
       </c>
       <c r="H5" s="10"/>
     </row>
@@ -10008,7 +10008,7 @@
       </c>
       <c r="G6" s="14">
         <f>G4-G5</f>
-        <v>586179965</v>
+        <v>586979965</v>
       </c>
       <c r="H6" s="10"/>
     </row>
@@ -10022,7 +10022,7 @@
       </c>
       <c r="G7" s="19">
         <f>G6/G4</f>
-        <v>0.652761653674833</v>
+        <v>0.653652522271715</v>
       </c>
       <c r="H7" s="10"/>
     </row>
@@ -10335,11 +10335,11 @@
       </c>
       <c r="E30" s="74"/>
       <c r="F30" s="71">
-        <v>8320035</v>
+        <v>7520035</v>
       </c>
       <c r="G30" s="71">
         <f>18000000-F30</f>
-        <v>9679965</v>
+        <v>10479965</v>
       </c>
       <c r="H30" s="10"/>
     </row>
@@ -10391,7 +10391,7 @@
       </c>
       <c r="E34" s="82"/>
       <c r="F34" s="83">
-        <v>21956248</v>
+        <v>21156248</v>
       </c>
       <c r="G34" s="84"/>
       <c r="H34" s="10"/>
@@ -10435,11 +10435,11 @@
       <c r="E37" s="93"/>
       <c r="F37" s="94">
         <f>F23+F34</f>
-        <v>311820035</v>
+        <v>311020035</v>
       </c>
       <c r="G37" s="95">
         <f>G4-F37</f>
-        <v>586179965</v>
+        <v>586979965</v>
       </c>
       <c r="H37" s="10"/>
       <c r="L37" s="71">

</xml_diff>